<commit_message>
feat: add quit button on main menu
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t xml:space="preserve">CRÉDITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAIN_QUIT_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUITTER</t>
   </si>
   <si>
     <t xml:space="preserve">CREDITS_TAGLINE</t>
@@ -303,10 +312,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -397,6 +406,17 @@
         <v>21</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(level): set the right order for levels then infinite loading
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t xml:space="preserve">QUITTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAIN_SEED_LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graine</t>
   </si>
   <si>
     <t xml:space="preserve">CREDITS_TAGLINE</t>
@@ -312,10 +321,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -417,6 +426,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(infinite): make infinite random configured by seed (#1)
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t xml:space="preserve">QUITTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAIN_SEED_LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graine</t>
   </si>
   <si>
     <t xml:space="preserve">CREDITS_TAGLINE</t>
@@ -312,10 +321,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -417,6 +426,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(level): make failure messaege more clear
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t xml:space="preserve">fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAIL_MESSAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You broke Linky!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous avez cassé Linky !</t>
   </si>
   <si>
     <t xml:space="preserve">GAME_NAME</t>
@@ -321,16 +330,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -351,23 +361,23 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -435,6 +445,17 @@
       </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>